<commit_message>
quitamos navegador de archivo externo, queda por linea de comando
</commit_message>
<xml_diff>
--- a/data/datos_qa.xlsx
+++ b/data/datos_qa.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fakku\OneDrive\Escritorio\Testing\Python\prueba\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fakku\OneDrive\Escritorio\Testing\Python\AutomatizacionPython\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E6EB09-835E-476C-8B08-85F83884B00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921D0A5A-B42A-45F9-B876-98AEEF1EB77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Entrada</t>
   </si>
@@ -34,15 +34,6 @@
   </si>
   <si>
     <t>python</t>
-  </si>
-  <si>
-    <t>navegador</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>edge</t>
   </si>
   <si>
     <t>tdd</t>
@@ -381,21 +372,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,66 +393,51 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>